<commit_message>
🤡 Ajout des views de l'application
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EF581B-D1CF-4C14-AA32-9A7970A41E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630F250F-ED8B-4B4E-8D62-5C4618F5082B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -1085,7 +1085,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2001,7 +2001,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2054,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 0 minutes</v>
+        <v>0 jours 2 heurs 20 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2073,11 +2073,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2219,15 +2219,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="str">
+      <c r="A11" s="16">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B11" s="50">
+        <v>45756</v>
+      </c>
       <c r="C11" s="51"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="52">
+        <v>20</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>30</v>
+      </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -8735,7 +8743,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8743,7 +8751,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8770,7 +8778,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>9.7222222222222224E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8793,17 +8801,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9026,6 +9023,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9035,17 +9043,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9062,4 +9059,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
➕ Ajout de Axios au dépendances
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630F250F-ED8B-4B4E-8D62-5C4618F5082B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F617FF5F-720D-4028-90A4-763D889D9459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Déplacer mon JDT et améliorer le README du projet</t>
+  </si>
+  <si>
+    <t>Création des views</t>
   </si>
 </sst>
 </file>
@@ -1070,7 +1073,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.472222222222222E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2001,7 +2004,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2057,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 20 minutes</v>
+        <v>0 jours 2 heurs 25 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2073,11 +2076,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2248,15 +2251,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B12" s="46">
+        <v>45756</v>
+      </c>
       <c r="C12" s="47"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="48">
+        <v>5</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>33</v>
+      </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -8603,7 +8614,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -8653,7 +8664,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8661,7 +8672,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8778,7 +8789,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>9.7222222222222224E-2</v>
+        <v>0.10069444444444445</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
💄 Ajout du header
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F617FF5F-720D-4028-90A4-763D889D9459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DA5604-DA49-4465-BF74-04C08F6FBADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Création des views</t>
+  </si>
+  <si>
+    <t>Header</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1076,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.472222222222222E-3</c:v>
+                  <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1088,7 +1091,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.5555555555555552E-2</c:v>
+                  <c:v>7.6388888888888895E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.0416666666666666E-2</c:v>
@@ -2004,7 +2007,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2057,7 +2060,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 25 minutes</v>
+        <v>0 jours 3 heurs 25 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2076,11 +2079,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>85</v>
+        <v>145</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2280,15 +2283,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B13" s="50">
+        <v>45756</v>
+      </c>
       <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="52">
+        <v>30</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>30</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2301,15 +2312,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B14" s="46">
+        <v>45756</v>
+      </c>
       <c r="C14" s="47"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="48">
+        <v>30</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -8664,7 +8683,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8672,7 +8691,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>3.472222222222222E-3</v>
+        <v>2.4305555555555556E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8754,7 +8773,7 @@
       </c>
       <c r="B10">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C10,'Journal de travail'!$D$7:$D$532)</f>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C10" s="37" t="str">
         <f>'Journal de travail'!M14</f>
@@ -8762,7 +8781,7 @@
       </c>
       <c r="D10" s="33">
         <f t="shared" si="0"/>
-        <v>5.5555555555555552E-2</v>
+        <v>7.6388888888888895E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -8789,7 +8808,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.10069444444444445</v>
+        <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8812,6 +8831,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9034,17 +9064,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9054,6 +9073,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9070,15 +9100,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
✨ Page d'accueil avec les livres en dur
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DA5604-DA49-4465-BF74-04C08F6FBADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F8B312-13D0-4676-BBB1-829883283181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="5085" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Header</t>
+  </si>
+  <si>
+    <t>Page d'accueil</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1079,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4305555555555556E-2</c:v>
+                  <c:v>4.5138888888888888E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2007,7 +2010,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2063,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 3 heurs 25 minutes</v>
+        <v>0 jours 3 heurs 55 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2079,11 +2082,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>145</v>
+        <v>175</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2341,15 +2344,23 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="str">
+      <c r="A15" s="16">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="50"/>
+        <v>15</v>
+      </c>
+      <c r="B15" s="50">
+        <v>45756</v>
+      </c>
       <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="36"/>
+      <c r="D15" s="52">
+        <v>30</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="G15" s="56"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -8683,7 +8694,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8691,7 +8702,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>2.4305555555555556E-2</v>
+        <v>4.5138888888888888E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8808,7 +8819,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.1423611111111111</v>
+        <v>0.16319444444444445</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8831,17 +8842,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9064,6 +9064,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9073,17 +9084,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9100,4 +9100,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
🚧 Services pour interroger le backend
CORS bloque la requête
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F8B312-13D0-4676-BBB1-829883283181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7E73EB-45E7-4F2F-891E-BB163630E2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="4620" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>Page d'accueil</t>
+  </si>
+  <si>
+    <t>Améliorer le style de la page d'accueil</t>
+  </si>
+  <si>
+    <t>Services pour la recherche par catégorie. Récupération des livres dans la homeView pour tester</t>
+  </si>
+  <si>
+    <t>CORS bloque la requête</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1088,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5138888888888888E-2</c:v>
+                  <c:v>0.1076388888888889</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2010,7 +2019,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2063,7 +2072,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 3 heurs 55 minutes</v>
+        <v>0 jours 5 heurs 25 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2078,15 +2087,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>235</v>
+        <v>325</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2373,31 +2382,49 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="46"/>
+        <v>18</v>
+      </c>
+      <c r="B16" s="46">
+        <v>45776</v>
+      </c>
       <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="48">
+        <v>30</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>36</v>
+      </c>
       <c r="G16" s="55"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
+        <v>18</v>
+      </c>
+      <c r="B17" s="50">
+        <v>45776</v>
+      </c>
+      <c r="C17" s="51">
+        <v>1</v>
+      </c>
       <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="56"/>
+      <c r="E17" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="56" t="s">
+        <v>38</v>
+      </c>
       <c r="O17">
         <v>45</v>
       </c>
@@ -8690,11 +8717,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8702,7 +8729,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>4.5138888888888888E-2</v>
+        <v>0.1076388888888889</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8819,7 +8846,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.16319444444444445</v>
+        <v>0.22569444444444445</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8842,6 +8869,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9064,17 +9102,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9084,6 +9111,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9100,15 +9138,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📝 JDT S2 Alban
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7E73EB-45E7-4F2F-891E-BB163630E2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C5A8FE-E5B7-4327-A587-101153E7A9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="4620" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>CORS bloque la requête</t>
+  </si>
+  <si>
+    <t>Récupérer les livres sur la page d'accueil. La mise en page est cassée</t>
+  </si>
+  <si>
+    <t>Début de la page de détails d'un livre. Le composant ne fonctionne pas: problème au niveau d'un props(null)</t>
   </si>
 </sst>
 </file>
@@ -1088,7 +1094,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1076388888888889</c:v>
+                  <c:v>0.19097222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2018,8 +2024,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2078,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 5 heurs 25 minutes</v>
+        <v>0 jours 7 heurs 25 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2087,7 +2093,7 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
@@ -2095,7 +2101,7 @@
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>325</v>
+        <v>445</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2430,30 +2436,46 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="str">
+      <c r="A18" s="8">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v/>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="47"/>
+        <v>18</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45777</v>
+      </c>
+      <c r="C18" s="47">
+        <v>1</v>
+      </c>
       <c r="D18" s="48"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="36"/>
+      <c r="E18" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="36" t="s">
+        <v>39</v>
+      </c>
       <c r="G18" s="55"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="str">
+    <row r="19" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v/>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="50">
+        <v>45777</v>
+      </c>
+      <c r="C19" s="51">
+        <v>1</v>
+      </c>
       <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="36"/>
+      <c r="E19" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G19" s="56"/>
       <c r="O19">
         <v>55</v>
@@ -8671,7 +8693,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -8717,7 +8739,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8729,7 +8751,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.1076388888888889</v>
+        <v>0.19097222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8846,7 +8868,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.22569444444444445</v>
+        <v>0.30902777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
📝 JDT S3 Alban
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C5A8FE-E5B7-4327-A587-101153E7A9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9907C388-A5E2-4DB7-8D76-C2796FADF42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="30360" yWindow="2880" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Autre</t>
   </si>
   <si>
-    <t>Nom Prénom</t>
-  </si>
-  <si>
     <t>18.03.2024  au 27.05.2024</t>
   </si>
   <si>
@@ -164,6 +161,36 @@
   </si>
   <si>
     <t>Début de la page de détails d'un livre. Le composant ne fonctionne pas: problème au niveau d'un props(null)</t>
+  </si>
+  <si>
+    <t>Centrer l'élément central de la page d'accueil</t>
+  </si>
+  <si>
+    <t>Segalen Alban</t>
+  </si>
+  <si>
+    <t>Ajout de l'image au seeder des livres</t>
+  </si>
+  <si>
+    <t>La route de récupération des détails d'un livre retourne le nombre de pages et le résumé</t>
+  </si>
+  <si>
+    <t>Récupérer les détails d'un livres et les affichers sur la page de détails</t>
+  </si>
+  <si>
+    <t>Animations sur l'image de la pgae de détails d'un livre</t>
+  </si>
+  <si>
+    <t>Ajouter la catégorie à la page de détails d'un livre</t>
+  </si>
+  <si>
+    <t>Récupération des commentaires et affichage sur la page de détails d'un livre</t>
+  </si>
+  <si>
+    <t>Journal de travail et export "gitTree"</t>
+  </si>
+  <si>
+    <t>Les livres sur la page d'accueil sont des liens vers leurs pages de détails</t>
   </si>
 </sst>
 </file>
@@ -1094,13 +1121,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19097222222222221</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0416666666666666E-2</c:v>
+                  <c:v>2.0833333333333332E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.0833333333333332E-2</c:v>
@@ -2024,8 +2051,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="6" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F533" sqref="F533"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="57"/>
@@ -2069,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
@@ -2078,7 +2105,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 25 minutes</v>
+        <v>0 jours 11 heurs 5 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2086,7 +2113,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="23.25" hidden="1" x14ac:dyDescent="0.35">
@@ -2097,11 +2124,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>205</v>
+        <v>425</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>445</v>
+        <v>665</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2120,19 +2147,19 @@
         <v>12</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2151,7 +2178,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="54"/>
     </row>
@@ -2171,7 +2198,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="55"/>
       <c r="M8" t="s">
@@ -2200,7 +2227,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="56"/>
       <c r="M9" t="s">
@@ -2229,7 +2256,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="55"/>
       <c r="M10" t="s">
@@ -2258,7 +2285,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="56"/>
       <c r="M11" t="s">
@@ -2287,7 +2314,7 @@
         <v>4</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
@@ -2316,7 +2343,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
@@ -2345,7 +2372,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
@@ -2374,7 +2401,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15" s="56"/>
       <c r="M15" t="s">
@@ -2403,7 +2430,7 @@
         <v>4</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16" s="55"/>
       <c r="O16">
@@ -2426,10 +2453,10 @@
         <v>4</v>
       </c>
       <c r="F17" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="56" t="s">
         <v>37</v>
-      </c>
-      <c r="G17" s="56" t="s">
-        <v>38</v>
       </c>
       <c r="O17">
         <v>45</v>
@@ -2451,7 +2478,7 @@
         <v>4</v>
       </c>
       <c r="F18" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="55"/>
       <c r="O18">
@@ -2474,7 +2501,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G19" s="56"/>
       <c r="O19">
@@ -2482,111 +2509,183 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="str">
+      <c r="A20" s="8">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v/>
-      </c>
-      <c r="B20" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="46">
+        <v>45783</v>
+      </c>
       <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="36"/>
+      <c r="D20" s="48">
+        <v>10</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="36" t="s">
+        <v>40</v>
+      </c>
       <c r="G20" s="55"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="str">
+      <c r="A21" s="16">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="50"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="50">
+        <v>45783</v>
+      </c>
       <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="36"/>
+      <c r="D21" s="52">
+        <v>10</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>42</v>
+      </c>
       <c r="G21" s="56"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="str">
+      <c r="A22" s="8">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="46">
+        <v>45783</v>
+      </c>
       <c r="C22" s="47"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="36"/>
+      <c r="D22" s="48">
+        <v>25</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>43</v>
+      </c>
       <c r="G22" s="55"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="str">
+      <c r="A23" s="16">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="50"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="50">
+        <v>45783</v>
+      </c>
       <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="36"/>
+      <c r="D23" s="52">
+        <v>50</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="G23" s="56"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="str">
+      <c r="A24" s="8">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="46">
+        <v>45783</v>
+      </c>
       <c r="C24" s="47"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="36"/>
+      <c r="D24" s="48">
+        <v>30</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>45</v>
+      </c>
       <c r="G24" s="55"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="str">
+      <c r="A25" s="16">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="50"/>
+        <v>19</v>
+      </c>
+      <c r="B25" s="50">
+        <v>45783</v>
+      </c>
       <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="36"/>
+      <c r="D25" s="52">
+        <v>20</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>46</v>
+      </c>
       <c r="G25" s="56"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="str">
+      <c r="A26" s="8">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B26" s="46">
+        <v>45783</v>
+      </c>
       <c r="C26" s="47"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="36"/>
+      <c r="D26" s="48">
+        <v>30</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>47</v>
+      </c>
       <c r="G26" s="55"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="str">
+      <c r="A27" s="16">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="50"/>
+        <v>19</v>
+      </c>
+      <c r="B27" s="50">
+        <v>45783</v>
+      </c>
       <c r="C27" s="51"/>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="36"/>
+      <c r="D27" s="52">
+        <v>30</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>49</v>
+      </c>
       <c r="G27" s="56"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="str">
+      <c r="A28" s="8">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="46"/>
+        <v>19</v>
+      </c>
+      <c r="B28" s="46">
+        <v>45783</v>
+      </c>
       <c r="C28" s="47"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="35"/>
+      <c r="D28" s="48">
+        <v>15</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>48</v>
+      </c>
       <c r="G28" s="55"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -8693,7 +8792,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -8743,7 +8842,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>95</v>
+        <v>300</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8751,7 +8850,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.19097222222222221</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8779,7 +8878,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8787,7 +8886,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8868,7 +8967,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.30902777777777779</v>
+        <v>0.46180555555555552</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
✨ On peut apprécier un livre
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA1A1C0-C347-49B8-BCF1-0AF99EEA5BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F245BCC8-7DD9-40F4-A570-E1D0B890FF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="2880" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="35130" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -203,6 +203,30 @@
   </si>
   <si>
     <t>JDT et export gitTree</t>
+  </si>
+  <si>
+    <t>Modification de la route de la récupération des livres pour avoir la possibilité de ne pas avoir de limite</t>
+  </si>
+  <si>
+    <t>Supprimmer le dossier application, la route GET /categorie/:id/livres et supprimmer la dépendance DevTools</t>
+  </si>
+  <si>
+    <t>Les services utilisent la même instance d'axios</t>
+  </si>
+  <si>
+    <t>Mettre à jour la route d'ajout d'un commentaire</t>
+  </si>
+  <si>
+    <t>Ajout du formulaire de commentaire à la page de détails d'un livre</t>
+  </si>
+  <si>
+    <t>Retour des notes et daily scrum</t>
+  </si>
+  <si>
+    <t>L'ajout d'un commentaire fonctionne, ils s'affichent directement après avoir été posté</t>
+  </si>
+  <si>
+    <t>Ajout des appréciations</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1157,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41666666666666669</c:v>
+                  <c:v>0.4236111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1142,7 +1166,7 @@
                   <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0833333333333332E-2</c:v>
+                  <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2063,8 +2087,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+      <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2117,7 +2141,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 13 heurs 20 minutes</v>
+        <v>0 jours 14 heurs 0 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2136,11 +2160,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>500</v>
+        <v>540</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>800</v>
+        <v>840</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2783,99 +2807,151 @@
       <c r="G32" s="55"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="str">
+      <c r="A33" s="16">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v/>
-      </c>
-      <c r="B33" s="50"/>
+        <v>20</v>
+      </c>
+      <c r="B33" s="50">
+        <v>45790</v>
+      </c>
       <c r="C33" s="51"/>
       <c r="D33" s="52"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="35"/>
+      <c r="E33" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>54</v>
+      </c>
       <c r="G33" s="56"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="str">
+      <c r="A34" s="8">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v/>
-      </c>
-      <c r="B34" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="B34" s="46">
+        <v>45790</v>
+      </c>
       <c r="C34" s="47"/>
       <c r="D34" s="48"/>
-      <c r="E34" s="49"/>
-      <c r="F34" s="35"/>
+      <c r="E34" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>55</v>
+      </c>
       <c r="G34" s="55"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="str">
+      <c r="A35" s="16">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v/>
-      </c>
-      <c r="B35" s="50"/>
+        <v>20</v>
+      </c>
+      <c r="B35" s="50">
+        <v>45790</v>
+      </c>
       <c r="C35" s="51"/>
       <c r="D35" s="52"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="36" t="s">
+        <v>56</v>
+      </c>
       <c r="G35" s="56"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="str">
+      <c r="A36" s="8">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v/>
-      </c>
-      <c r="B36" s="46"/>
+        <v>20</v>
+      </c>
+      <c r="B36" s="46">
+        <v>45790</v>
+      </c>
       <c r="C36" s="47"/>
       <c r="D36" s="48"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="35"/>
+      <c r="E36" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>57</v>
+      </c>
       <c r="G36" s="55"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="str">
+      <c r="A37" s="16">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v/>
-      </c>
-      <c r="B37" s="50"/>
+        <v>20</v>
+      </c>
+      <c r="B37" s="50">
+        <v>45790</v>
+      </c>
       <c r="C37" s="51"/>
       <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>58</v>
+      </c>
       <c r="G37" s="56"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="str">
+      <c r="A38" s="8">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
-        <v/>
-      </c>
-      <c r="B38" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B38" s="46">
+        <v>45797</v>
+      </c>
       <c r="C38" s="47"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="35"/>
+      <c r="D38" s="48">
+        <v>30</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>59</v>
+      </c>
       <c r="G38" s="55"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="str">
+      <c r="A39" s="16">
         <f>IF(ISBLANK(B39),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B39))</f>
-        <v/>
-      </c>
-      <c r="B39" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B39" s="50">
+        <v>45797</v>
+      </c>
       <c r="C39" s="51"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="35"/>
+      <c r="D39" s="52">
+        <v>10</v>
+      </c>
+      <c r="E39" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>60</v>
+      </c>
       <c r="G39" s="56"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="str">
+      <c r="A40" s="8">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v/>
-      </c>
-      <c r="B40" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B40" s="46">
+        <v>45797</v>
+      </c>
       <c r="C40" s="47"/>
       <c r="D40" s="48"/>
-      <c r="E40" s="49"/>
-      <c r="F40" s="35"/>
+      <c r="E40" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>61</v>
+      </c>
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -8888,7 +8964,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8896,7 +8972,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.41666666666666669</v>
+        <v>0.4236111111111111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8942,7 +9018,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -8950,7 +9026,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9013,7 +9089,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.55555555555555558</v>
+        <v>0.58333333333333348</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
📝 JDT Alban 20.05.25
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F245BCC8-7DD9-40F4-A570-E1D0B890FF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5484F438-0688-4AF3-82BD-34A5E475C431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="35130" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -228,6 +228,21 @@
   <si>
     <t>Ajout des appréciations</t>
   </si>
+  <si>
+    <t>Si on a apprécié un livre, l'appréciation est récupérée et affichée</t>
+  </si>
+  <si>
+    <t>Supprimer le paramètre user_id lors de l'ajout d'un commentaire</t>
+  </si>
+  <si>
+    <t>Ajout du pied-de-page</t>
+  </si>
+  <si>
+    <t>Modifier le script de démarrage pour qu'il ouvre le CDC</t>
+  </si>
+  <si>
+    <t>Problèmes avec git. Des problèmes aparaissent lorsqu'on change on fichier binaire (le JDT) de branche, ce qui m'a ralenti dans mon travail, et qui m'a obligé à refaire une partie du JDT</t>
+  </si>
 </sst>
 </file>
 
@@ -410,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -545,6 +560,10 @@
     </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1157,7 +1176,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4236111111111111</c:v>
+                  <c:v>0.67013888888888884</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1166,7 +1185,7 @@
                   <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>4.8611111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1175,7 +1194,7 @@
                   <c:v>7.6388888888888895E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7361111111111112E-2</c:v>
+                  <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2087,8 +2106,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <pane ySplit="6" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2141,7 +2160,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 0 minutes</v>
+        <v>0 jours 20 heurs 30 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2156,15 +2175,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>540</v>
+        <v>810</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>840</v>
+        <v>1230</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2814,7 +2833,9 @@
       <c r="B33" s="50">
         <v>45790</v>
       </c>
-      <c r="C33" s="51"/>
+      <c r="C33" s="51">
+        <v>1</v>
+      </c>
       <c r="D33" s="52"/>
       <c r="E33" s="53" t="s">
         <v>4</v>
@@ -2833,7 +2854,9 @@
         <v>45790</v>
       </c>
       <c r="C34" s="47"/>
-      <c r="D34" s="48"/>
+      <c r="D34" s="48">
+        <v>20</v>
+      </c>
       <c r="E34" s="49" t="s">
         <v>4</v>
       </c>
@@ -2851,7 +2874,9 @@
         <v>45790</v>
       </c>
       <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
+      <c r="D35" s="52">
+        <v>30</v>
+      </c>
       <c r="E35" s="53" t="s">
         <v>4</v>
       </c>
@@ -2869,7 +2894,9 @@
         <v>45790</v>
       </c>
       <c r="C36" s="47"/>
-      <c r="D36" s="48"/>
+      <c r="D36" s="48">
+        <v>45</v>
+      </c>
       <c r="E36" s="49" t="s">
         <v>4</v>
       </c>
@@ -2886,7 +2913,9 @@
       <c r="B37" s="50">
         <v>45790</v>
       </c>
-      <c r="C37" s="51"/>
+      <c r="C37" s="51">
+        <v>1</v>
+      </c>
       <c r="D37" s="52"/>
       <c r="E37" s="53" t="s">
         <v>4</v>
@@ -2906,7 +2935,7 @@
       </c>
       <c r="C38" s="47"/>
       <c r="D38" s="48">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E38" s="49" t="s">
         <v>7</v>
@@ -2926,7 +2955,7 @@
       </c>
       <c r="C39" s="51"/>
       <c r="D39" s="52">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E39" s="53" t="s">
         <v>4</v>
@@ -2945,7 +2974,9 @@
         <v>45797</v>
       </c>
       <c r="C40" s="47"/>
-      <c r="D40" s="48"/>
+      <c r="D40" s="48">
+        <v>45</v>
+      </c>
       <c r="E40" s="49" t="s">
         <v>4</v>
       </c>
@@ -2955,63 +2986,103 @@
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="str">
+      <c r="A41" s="16">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B41" s="50">
+        <v>45797</v>
+      </c>
       <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="35"/>
+      <c r="D41" s="52">
+        <v>35</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>62</v>
+      </c>
       <c r="G41" s="56"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="str">
+      <c r="A42" s="8">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B42" s="46">
+        <v>45797</v>
+      </c>
       <c r="C42" s="47"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="35"/>
+      <c r="D42" s="48">
+        <v>15</v>
+      </c>
+      <c r="E42" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>63</v>
+      </c>
       <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="str">
+      <c r="A43" s="16">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B43" s="50">
+        <v>45797</v>
+      </c>
       <c r="C43" s="51"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="35"/>
+      <c r="D43" s="52">
+        <v>30</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>64</v>
+      </c>
       <c r="G43" s="56"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="str">
+      <c r="A44" s="8">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B44" s="46">
+        <v>45797</v>
+      </c>
       <c r="C44" s="47"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="35"/>
+      <c r="D44" s="48">
+        <v>5</v>
+      </c>
+      <c r="E44" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>65</v>
+      </c>
       <c r="G44" s="55"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="str">
+      <c r="A45" s="16">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B45" s="50">
+        <v>45797</v>
+      </c>
       <c r="C45" s="51"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="35"/>
+      <c r="D45" s="52">
+        <v>20</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>66</v>
+      </c>
       <c r="G45" s="56"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3035,7 +3106,7 @@
       <c r="C47" s="51"/>
       <c r="D47" s="52"/>
       <c r="E47" s="53"/>
-      <c r="F47" s="35"/>
+      <c r="F47" s="59"/>
       <c r="G47" s="56"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -8960,11 +9031,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>370</v>
+        <v>605</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8972,7 +9043,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.4236111111111111</v>
+        <v>0.67013888888888884</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9018,7 +9089,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -9026,7 +9097,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9072,7 +9143,7 @@
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -9080,7 +9151,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -9089,7 +9160,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.58333333333333348</v>
+        <v>0.85416666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9112,6 +9183,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9334,17 +9416,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9354,6 +9425,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9370,15 +9452,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
✨ On peut ajouter, modifier et supprimer une appréciation
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F245BCC8-7DD9-40F4-A570-E1D0B890FF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CE9D42-BD94-4FF9-8455-62440ED55343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="35130" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>Ajout des appréciations</t>
+  </si>
+  <si>
+    <t>Daily Scrum</t>
+  </si>
+  <si>
+    <t>Modification de la route put /appreciations/:id pour créer l'appréciation si elle n'existe pas et la modifier sinon</t>
+  </si>
+  <si>
+    <t>Modifier la route de supression d'une appréciation pour ne pas utiliser l'id de l'appréciation, mais livre_fk et utilisateur_fk</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1166,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4236111111111111</c:v>
+                  <c:v>0.4861111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1166,7 +1175,7 @@
                   <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>4.8611111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2087,8 +2096,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2141,7 +2150,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 14 heurs 0 minutes</v>
+        <v>0 jours 15 heurs 40 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2156,15 +2165,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>540</v>
+        <v>580</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>840</v>
+        <v>940</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2955,39 +2964,63 @@
       <c r="G40" s="55"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="str">
+      <c r="A41" s="16">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v/>
-      </c>
-      <c r="B41" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B41" s="50">
+        <v>45798</v>
+      </c>
       <c r="C41" s="51"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="35"/>
+      <c r="D41" s="52">
+        <v>10</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>62</v>
+      </c>
       <c r="G41" s="56"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="str">
+      <c r="A42" s="8">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v/>
-      </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="47"/>
+        <v>21</v>
+      </c>
+      <c r="B42" s="46">
+        <v>45798</v>
+      </c>
+      <c r="C42" s="47">
+        <v>1</v>
+      </c>
       <c r="D42" s="48"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="35"/>
+      <c r="E42" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="35" t="s">
+        <v>63</v>
+      </c>
       <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="str">
+      <c r="A43" s="16">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v/>
-      </c>
-      <c r="B43" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B43" s="50">
+        <v>45798</v>
+      </c>
       <c r="C43" s="51"/>
-      <c r="D43" s="52"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="35"/>
+      <c r="D43" s="52">
+        <v>30</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="35" t="s">
+        <v>64</v>
+      </c>
       <c r="G43" s="56"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -8960,11 +8993,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>370</v>
+        <v>400</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8972,7 +9005,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.4236111111111111</v>
+        <v>0.4861111111111111</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9018,7 +9051,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -9026,7 +9059,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>4.8611111111111112E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9089,7 +9122,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.58333333333333348</v>
+        <v>0.6527777777777779</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9112,6 +9145,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9334,17 +9378,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -9354,6 +9387,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9370,15 +9414,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📝 Réparation du JDT Alban 😡
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CE9D42-BD94-4FF9-8455-62440ED55343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0DB206-0080-4481-BCC7-42700E4F1003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="15" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -229,13 +229,28 @@
     <t>Ajout des appréciations</t>
   </si>
   <si>
-    <t>Daily Scrum</t>
+    <t>Si on a apprécié un livre, l'appréciation est récupérée et affichée</t>
+  </si>
+  <si>
+    <t>Supprimer le paramètre user_id lors de l'ajout d'un commentaire</t>
+  </si>
+  <si>
+    <t>Ajout du pied-de-page</t>
+  </si>
+  <si>
+    <t>Modifier le script de démarrage pour qu'il ouvre le CDC</t>
+  </si>
+  <si>
+    <t>Problèmes avec git. Des problèmes aparaissent lorsqu'on change on fichier binaire (le JDT) de branche, ce qui m'a ralenti dans mon travail, et qui m'a obligé à refaire une partie du JDT</t>
   </si>
   <si>
     <t>Modification de la route put /appreciations/:id pour créer l'appréciation si elle n'existe pas et la modifier sinon</t>
   </si>
   <si>
     <t>Modifier la route de supression d'une appréciation pour ne pas utiliser l'id de l'appréciation, mais livre_fk et utilisateur_fk</t>
+  </si>
+  <si>
+    <t>Daily Scrum</t>
   </si>
 </sst>
 </file>
@@ -419,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -546,6 +561,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1166,7 +1185,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4861111111111111</c:v>
+                  <c:v>0.73263888888888884</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1175,7 +1194,7 @@
                   <c:v>2.4305555555555556E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8611111111111112E-2</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1184,7 +1203,7 @@
                   <c:v>7.6388888888888895E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7361111111111112E-2</c:v>
+                  <c:v>3.4722222222222224E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2097,7 +2116,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2132,11 +2151,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2150,7 +2169,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 15 heurs 40 minutes</v>
+        <v>0 jours 22 heurs 10 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2165,24 +2184,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>580</v>
+        <v>850</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>940</v>
+        <v>1330</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="58" t="s">
+      <c r="C5" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="58"/>
+      <c r="D5" s="59"/>
     </row>
     <row r="6" spans="1:15" s="20" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
@@ -2823,7 +2842,9 @@
       <c r="B33" s="50">
         <v>45790</v>
       </c>
-      <c r="C33" s="51"/>
+      <c r="C33" s="51">
+        <v>1</v>
+      </c>
       <c r="D33" s="52"/>
       <c r="E33" s="53" t="s">
         <v>4</v>
@@ -2842,7 +2863,9 @@
         <v>45790</v>
       </c>
       <c r="C34" s="47"/>
-      <c r="D34" s="48"/>
+      <c r="D34" s="48">
+        <v>20</v>
+      </c>
       <c r="E34" s="49" t="s">
         <v>4</v>
       </c>
@@ -2860,7 +2883,9 @@
         <v>45790</v>
       </c>
       <c r="C35" s="51"/>
-      <c r="D35" s="52"/>
+      <c r="D35" s="52">
+        <v>30</v>
+      </c>
       <c r="E35" s="53" t="s">
         <v>4</v>
       </c>
@@ -2878,7 +2903,9 @@
         <v>45790</v>
       </c>
       <c r="C36" s="47"/>
-      <c r="D36" s="48"/>
+      <c r="D36" s="48">
+        <v>45</v>
+      </c>
       <c r="E36" s="49" t="s">
         <v>4</v>
       </c>
@@ -2895,7 +2922,9 @@
       <c r="B37" s="50">
         <v>45790</v>
       </c>
-      <c r="C37" s="51"/>
+      <c r="C37" s="51">
+        <v>1</v>
+      </c>
       <c r="D37" s="52"/>
       <c r="E37" s="53" t="s">
         <v>4</v>
@@ -2915,7 +2944,7 @@
       </c>
       <c r="C38" s="47"/>
       <c r="D38" s="48">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E38" s="49" t="s">
         <v>7</v>
@@ -2935,7 +2964,7 @@
       </c>
       <c r="C39" s="51"/>
       <c r="D39" s="52">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E39" s="53" t="s">
         <v>4</v>
@@ -2954,7 +2983,9 @@
         <v>45797</v>
       </c>
       <c r="C40" s="47"/>
-      <c r="D40" s="48"/>
+      <c r="D40" s="48">
+        <v>45</v>
+      </c>
       <c r="E40" s="49" t="s">
         <v>4</v>
       </c>
@@ -2969,14 +3000,14 @@
         <v>21</v>
       </c>
       <c r="B41" s="50">
-        <v>45798</v>
+        <v>45797</v>
       </c>
       <c r="C41" s="51"/>
       <c r="D41" s="52">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E41" s="53" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F41" s="35" t="s">
         <v>62</v>
@@ -2989,12 +3020,12 @@
         <v>21</v>
       </c>
       <c r="B42" s="46">
-        <v>45798</v>
-      </c>
-      <c r="C42" s="47">
-        <v>1</v>
-      </c>
-      <c r="D42" s="48"/>
+        <v>45797</v>
+      </c>
+      <c r="C42" s="47"/>
+      <c r="D42" s="48">
+        <v>15</v>
+      </c>
       <c r="E42" s="49" t="s">
         <v>4</v>
       </c>
@@ -3009,7 +3040,7 @@
         <v>21</v>
       </c>
       <c r="B43" s="50">
-        <v>45798</v>
+        <v>45797</v>
       </c>
       <c r="C43" s="51"/>
       <c r="D43" s="52">
@@ -3024,63 +3055,103 @@
       <c r="G43" s="56"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="str">
+      <c r="A44" s="8">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v/>
-      </c>
-      <c r="B44" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B44" s="46">
+        <v>45797</v>
+      </c>
       <c r="C44" s="47"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="35"/>
+      <c r="D44" s="48">
+        <v>5</v>
+      </c>
+      <c r="E44" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>65</v>
+      </c>
       <c r="G44" s="55"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="str">
+      <c r="A45" s="16">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v/>
-      </c>
-      <c r="B45" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B45" s="50">
+        <v>45797</v>
+      </c>
       <c r="C45" s="51"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="35"/>
+      <c r="D45" s="52">
+        <v>20</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>66</v>
+      </c>
       <c r="G45" s="56"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="str">
+      <c r="A46" s="8">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v/>
-      </c>
-      <c r="B46" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B46" s="46">
+        <v>45798</v>
+      </c>
       <c r="C46" s="47"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="35"/>
+      <c r="D46" s="48">
+        <v>10</v>
+      </c>
+      <c r="E46" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="35" t="s">
+        <v>69</v>
+      </c>
       <c r="G46" s="55"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="str">
+      <c r="A47" s="16">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v/>
-      </c>
-      <c r="B47" s="50"/>
-      <c r="C47" s="51"/>
+        <v>21</v>
+      </c>
+      <c r="B47" s="50">
+        <v>45798</v>
+      </c>
+      <c r="C47" s="51">
+        <v>1</v>
+      </c>
       <c r="D47" s="52"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="35"/>
+      <c r="E47" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="57" t="s">
+        <v>67</v>
+      </c>
       <c r="G47" s="56"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="str">
+      <c r="A48" s="8">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v/>
-      </c>
-      <c r="B48" s="46"/>
+        <v>21</v>
+      </c>
+      <c r="B48" s="46">
+        <v>45798</v>
+      </c>
       <c r="C48" s="47"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="35"/>
+      <c r="D48" s="48">
+        <v>30</v>
+      </c>
+      <c r="E48" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="35" t="s">
+        <v>68</v>
+      </c>
       <c r="G48" s="55"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -8993,11 +9064,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>400</v>
+        <v>635</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9005,7 +9076,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.4861111111111111</v>
+        <v>0.73263888888888884</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9051,7 +9122,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>'Journal de travail'!M12</f>
@@ -9059,7 +9130,7 @@
       </c>
       <c r="D8" s="33">
         <f t="shared" si="0"/>
-        <v>4.8611111111111112E-2</v>
+        <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -9105,7 +9176,7 @@
       </c>
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C11" s="39" t="str">
         <f>'Journal de travail'!M15</f>
@@ -9113,7 +9184,7 @@
       </c>
       <c r="D11" s="33">
         <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -9122,7 +9193,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.6527777777777779</v>
+        <v>0.92361111111111105</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9136,26 +9207,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9378,10 +9429,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9398,20 +9480,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📝 JDT Alban 21.05.25
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0DB206-0080-4481-BCC7-42700E4F1003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB25BF7-E220-41F0-A926-84C53F586B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="33375" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>Daily Scrum</t>
+  </si>
+  <si>
+    <t>Affichage de la moyenne de la note du livre. WIP</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1188,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73263888888888884</c:v>
+                  <c:v>0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2115,8 +2118,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+      <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2169,7 +2172,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 22 heurs 10 minutes</v>
+        <v>0 jours 23 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2188,11 +2191,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>850</v>
+        <v>915</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>1330</v>
+        <v>1395</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -3125,7 +3128,9 @@
       <c r="C47" s="51">
         <v>1</v>
       </c>
-      <c r="D47" s="52"/>
+      <c r="D47" s="52">
+        <v>20</v>
+      </c>
       <c r="E47" s="53" t="s">
         <v>4</v>
       </c>
@@ -3155,15 +3160,23 @@
       <c r="G48" s="55"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="16" t="str">
+      <c r="A49" s="16">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B49))</f>
-        <v/>
-      </c>
-      <c r="B49" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B49" s="50">
+        <v>45798</v>
+      </c>
       <c r="C49" s="51"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="35"/>
+      <c r="D49" s="52">
+        <v>45</v>
+      </c>
+      <c r="E49" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>70</v>
+      </c>
       <c r="G49" s="56"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -9005,8 +9018,8 @@
       <formula1>$M$7:$M$15</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="80" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -9068,7 +9081,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>635</v>
+        <v>700</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9076,7 +9089,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.73263888888888884</v>
+        <v>0.77777777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9193,7 +9206,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.92361111111111105</v>
+        <v>0.96875000000000011</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
📝 JDT 27.05.25 Alban
</commit_message>
<xml_diff>
--- a/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
+++ b/frontend/Journal_de_Travail/Journal-de-Travail_SegalenAlban.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po37sqb\Documents\GitHub\P_Web295\frontend\Journal_de_Travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB25BF7-E220-41F0-A926-84C53F586B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86284ED7-9A55-48A5-A61B-9F5F674318D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="33375" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="31995" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -254,6 +254,12 @@
   </si>
   <si>
     <t>Affichage de la moyenne de la note du livre. WIP</t>
+  </si>
+  <si>
+    <t>Faire en sorte que les appréciations soient entre 0 et 5</t>
+  </si>
+  <si>
+    <t>Cacher le formulaire de commentaire si l'utilisateur n'est pas connecté</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1194,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77777777777777779</c:v>
+                  <c:v>0.79861111111111116</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2119,7 +2125,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2172,7 +2178,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 23 heurs 15 minutes</v>
+        <v>0 jours 23 heurs 45 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2191,11 +2197,11 @@
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>915</v>
+        <v>945</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>1395</v>
+        <v>1425</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -3180,27 +3186,43 @@
       <c r="G49" s="56"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="str">
+      <c r="A50" s="8">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B50))</f>
-        <v/>
-      </c>
-      <c r="B50" s="46"/>
+        <v>22</v>
+      </c>
+      <c r="B50" s="46">
+        <v>45804</v>
+      </c>
       <c r="C50" s="47"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="35"/>
+      <c r="D50" s="48">
+        <v>10</v>
+      </c>
+      <c r="E50" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>71</v>
+      </c>
       <c r="G50" s="55"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="str">
+      <c r="A51" s="16">
         <f>IF(ISBLANK(B51),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B51))</f>
-        <v/>
-      </c>
-      <c r="B51" s="50"/>
+        <v>22</v>
+      </c>
+      <c r="B51" s="50">
+        <v>45804</v>
+      </c>
       <c r="C51" s="51"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="35"/>
+      <c r="D51" s="52">
+        <v>20</v>
+      </c>
+      <c r="E51" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="35" t="s">
+        <v>72</v>
+      </c>
       <c r="G51" s="56"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -9081,7 +9103,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>700</v>
+        <v>730</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9089,7 +9111,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.77777777777777779</v>
+        <v>0.79861111111111116</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -9206,7 +9228,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.96875000000000011</v>
+        <v>0.98958333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9443,6 +9465,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9451,15 +9482,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9482,6 +9504,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9490,12 +9520,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>